<commit_message>
Added new Quality target which went missing but was in the requirements and the rating matrix. Corrected some Errorscenarions for the external interfaces. Removed unrated cirtria from the xlsx and the katalog in the SAD.
</commit_message>
<xml_diff>
--- a/Bewertungsmatrix-v1.xlsx
+++ b/Bewertungsmatrix-v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="6120" windowWidth="24760" windowHeight="16440"/>
+    <workbookView xWindow="2100" yWindow="6120" windowWidth="20400" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Nr</t>
   </si>
@@ -78,9 +78,6 @@
     <t>BK11</t>
   </si>
   <si>
-    <t>BK12</t>
-  </si>
-  <si>
     <t>Lernkurve</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Docker Compose,Swarm</t>
   </si>
   <si>
-    <t>Kubernetes</t>
-  </si>
-  <si>
     <t>SaltStack</t>
   </si>
   <si>
@@ -195,22 +189,16 @@
     <t>Lizenzkosten</t>
   </si>
   <si>
-    <t>Interportabilität</t>
-  </si>
-  <si>
     <t>Strategisch</t>
   </si>
   <si>
     <t>Know-How</t>
   </si>
   <si>
-    <t>BK13</t>
-  </si>
-  <si>
-    <t>Muli Version</t>
-  </si>
-  <si>
     <t>Konfigurationsänderung / Neustart</t>
+  </si>
+  <si>
+    <t>OpenShift</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1014,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:R16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:R14" totalsRowShown="0">
   <tableColumns count="18">
     <tableColumn id="1" name="Nr" dataDxfId="33"/>
     <tableColumn id="2" name="Beschreibung" dataDxfId="32" totalsRowDxfId="31"/>
@@ -1043,7 +1031,7 @@
     <tableColumn id="18" name="Mesage-Queue Redis" dataDxfId="11" totalsRowDxfId="10"/>
     <tableColumn id="25" name="Spring-Rest" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="24" name="Docker Compose,Swarm" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="23" name="Kubernetes" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="23" name="OpenShift" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="22" name="SaltStack" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="26" name="Spring Cloud Config" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
@@ -1348,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1374,7 +1362,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1399,24 +1387,24 @@
       <c r="B2" s="45"/>
       <c r="C2" s="46"/>
       <c r="D2" s="39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="40"/>
       <c r="F2" s="40"/>
       <c r="G2" s="41"/>
       <c r="H2" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="40"/>
       <c r="J2" s="40"/>
       <c r="K2" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L2" s="40"/>
       <c r="M2" s="40"/>
       <c r="N2" s="41"/>
       <c r="O2" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P2" s="43"/>
       <c r="Q2" s="43"/>
@@ -1430,52 +1418,52 @@
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="L3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="M3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="N3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="O3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="P3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="18" t="s">
+      <c r="R3" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -1483,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -1533,7 +1521,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -1583,7 +1571,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -1667,7 +1655,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
@@ -1717,7 +1705,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -1812,41 +1800,65 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
-        <v>3</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3</v>
+      </c>
+      <c r="G11" s="8">
+        <v>5</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="8"/>
+      <c r="K11" s="7">
+        <v>3</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11" s="5">
+        <v>3</v>
+      </c>
+      <c r="N11" s="8">
+        <v>5</v>
+      </c>
+      <c r="O11" s="7">
+        <v>4</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>1</v>
+      </c>
+      <c r="R11" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="7">
         <v>5</v>
@@ -1855,57 +1867,41 @@
         <v>4</v>
       </c>
       <c r="F12" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="7">
-        <v>3</v>
-      </c>
-      <c r="L12" s="4">
-        <v>2</v>
-      </c>
-      <c r="M12" s="5">
-        <v>3</v>
-      </c>
-      <c r="N12" s="8">
-        <v>5</v>
-      </c>
-      <c r="O12" s="7">
-        <v>4</v>
-      </c>
-      <c r="P12" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>1</v>
-      </c>
-      <c r="R12" s="8">
-        <v>5</v>
-      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="8"/>
     </row>
     <row r="13" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13" s="7">
         <v>5</v>
       </c>
       <c r="E13" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="8">
         <v>1</v>
@@ -1913,245 +1909,229 @@
       <c r="H13" s="7"/>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="8"/>
-    </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="7">
+        <v>2</v>
+      </c>
+      <c r="L13" s="4">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5">
+        <v>2</v>
+      </c>
+      <c r="N13" s="8">
+        <v>5</v>
+      </c>
+      <c r="O13" s="7">
+        <v>1</v>
+      </c>
+      <c r="P13" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>5</v>
+      </c>
+      <c r="R13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
-      <c r="F14" s="5">
-        <v>2</v>
-      </c>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="7">
-        <v>2</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5">
-        <v>2</v>
-      </c>
-      <c r="N14" s="8">
-        <v>5</v>
-      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="8"/>
       <c r="O14" s="7">
         <v>1</v>
       </c>
       <c r="P14" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q14" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="3" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="9">
+        <f>SUMPRODUCT(C4:C14,D4:D14)</f>
+        <v>158</v>
+      </c>
+      <c r="E15" s="10">
+        <f>SUMPRODUCT(C4:C14,E4:E14)</f>
+        <v>136</v>
+      </c>
+      <c r="F15" s="11">
+        <f>SUMPRODUCT(C4:C14,F4:F14)</f>
+        <v>116</v>
+      </c>
+      <c r="G15" s="12">
+        <f>SUMPRODUCT(C4:C14,G4:G14)</f>
+        <v>122</v>
+      </c>
+      <c r="H15" s="13">
+        <f>SUMPRODUCT(C4:C14,H4:H14)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="10">
+        <f>SUMPRODUCT(C4:C14,I4:I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <f>SUMPRODUCT(C4:C14,J4:J14)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <f>SUMPRODUCT(C4:C14,K4:K14)</f>
+        <v>121</v>
+      </c>
+      <c r="L15" s="10">
+        <f>SUMPRODUCT(C4:C14,L4:L14)</f>
+        <v>123</v>
+      </c>
+      <c r="M15" s="11">
+        <f>SUMPRODUCT(C4:C14,M4:M14)</f>
+        <v>126</v>
+      </c>
+      <c r="N15" s="12">
+        <f>SUMPRODUCT(C4:C14,N4:N14)</f>
+        <v>147</v>
+      </c>
+      <c r="O15" s="13">
+        <f>SUMPRODUCT(C4:C14,O4:O14)</f>
+        <v>89</v>
+      </c>
+      <c r="P15" s="10">
+        <f>SUMPRODUCT(C4:C14,P4:P14)</f>
+        <v>112</v>
+      </c>
+      <c r="Q15" s="11">
+        <f>SUMPRODUCT(C4:C14,Q4:Q14)</f>
+        <v>125</v>
+      </c>
+      <c r="R15" s="12">
+        <f>SUMPRODUCT(C4:C14,R4:R14)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+    </row>
+    <row r="17" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="O17" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="36"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="15">
         <v>2</v>
       </c>
-      <c r="E15" s="4">
-        <v>2</v>
-      </c>
-      <c r="F15" s="5">
-        <v>4</v>
-      </c>
-      <c r="G15" s="8">
-        <v>4</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="8"/>
-    </row>
-    <row r="16" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="7">
-        <v>1</v>
-      </c>
-      <c r="P16" s="4">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>1</v>
-      </c>
-      <c r="R16" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" s="3" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="9">
-        <f>SUMPRODUCT(C4:C16,D4:D16)</f>
-        <v>168</v>
-      </c>
-      <c r="E17" s="10">
-        <f>SUMPRODUCT(C4:C16,E4:E16)</f>
-        <v>146</v>
-      </c>
-      <c r="F17" s="11">
-        <f>SUMPRODUCT(C4:C16,F4:F16)</f>
-        <v>136</v>
-      </c>
-      <c r="G17" s="12">
-        <f>SUMPRODUCT(C4:C16,G4:G16)</f>
-        <v>142</v>
-      </c>
-      <c r="H17" s="13">
-        <f>SUMPRODUCT(C4:C16,H4:H16)</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="10">
-        <f>SUMPRODUCT(C4:C16,I4:I16)</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="11">
-        <f>SUMPRODUCT(C4:C16,J4:J16)</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="13">
-        <f>SUMPRODUCT(C4:C16,K4:K16)</f>
-        <v>121</v>
-      </c>
-      <c r="L17" s="10">
-        <f>SUMPRODUCT(C4:C16,L4:L16)</f>
-        <v>123</v>
-      </c>
-      <c r="M17" s="11">
-        <f>SUMPRODUCT(C4:C16,M4:M16)</f>
-        <v>126</v>
-      </c>
-      <c r="N17" s="12">
-        <f>SUMPRODUCT(C4:C16,N4:N16)</f>
-        <v>147</v>
-      </c>
-      <c r="O17" s="13">
-        <f>SUMPRODUCT(C4:C16,O4:O16)</f>
-        <v>89</v>
-      </c>
-      <c r="P17" s="10">
-        <f>SUMPRODUCT(C4:C16,P4:P16)</f>
-        <v>112</v>
-      </c>
-      <c r="Q17" s="11">
-        <f>SUMPRODUCT(C4:C16,Q4:Q16)</f>
-        <v>125</v>
-      </c>
-      <c r="R17" s="12">
-        <f>SUMPRODUCT(C4:C16,R4:R16)</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-    </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
+      <c r="O18" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="36"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="27"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="30"/>
       <c r="N19" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P19" s="35"/>
       <c r="Q19" s="35"/>
@@ -2165,7 +2145,7 @@
       <c r="E20" s="29"/>
       <c r="F20" s="30"/>
       <c r="G20" s="22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
@@ -2174,10 +2154,10 @@
       <c r="L20" s="29"/>
       <c r="M20" s="30"/>
       <c r="N20" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O20" s="34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P20" s="35"/>
       <c r="Q20" s="35"/>
@@ -2187,86 +2167,40 @@
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="30"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
       <c r="N21" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O21" s="34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P21" s="35"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="36"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="15">
-        <v>4</v>
-      </c>
-      <c r="O22" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="36"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="15">
-        <v>5</v>
-      </c>
-      <c r="O23" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="36"/>
+      <c r="A23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="3"/>
+      <c r="A24" s="14"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
-      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
@@ -2274,30 +2208,24 @@
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J34" s="14"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J32" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A18:R18"/>
+    <mergeCell ref="A16:R16"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="O18:R18"/>
     <mergeCell ref="O19:R19"/>
     <mergeCell ref="O20:R20"/>
     <mergeCell ref="O21:R21"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="O23:R23"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>